<commit_message>
Scripting SCD0179 - Validasi Field Report PHR Pada Searching Portal/Action0/ObjectRepository and SCD0180 - Sales Mengakses Menu Report - Menu Product Holding Ratio - Report
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0175_Penambahan Leads dari Store ke Cart.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0175_Penambahan Leads dari Store ke Cart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0176A45-9004-4C2E-BD2A-5F9C68DEFD21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9462CC-108B-4264-A6EA-C8E5FE5EF46F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -98,16 +98,16 @@
     <t>Kelolaan</t>
   </si>
   <si>
-    <t>ade</t>
-  </si>
-  <si>
-    <t>contoh uft</t>
-  </si>
-  <si>
-    <t>nadia 6</t>
-  </si>
-  <si>
-    <t>isty 5</t>
+    <t>nadia 2</t>
+  </si>
+  <si>
+    <t>dewi 8</t>
+  </si>
+  <si>
+    <t>tyas</t>
+  </si>
+  <si>
+    <t>bnimf</t>
   </si>
 </sst>
 </file>
@@ -515,7 +515,7 @@
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,7 +614,7 @@
       </c>
       <c r="K2" s="7"/>
       <c r="L2" s="12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="M2" s="15" t="s">
         <v>22</v>
@@ -658,7 +658,7 @@
       </c>
       <c r="K3" s="7"/>
       <c r="L3" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M3" s="15" t="s">
         <v>22</v>
@@ -699,7 +699,7 @@
       </c>
       <c r="K4" s="7"/>
       <c r="L4" s="12" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="M4" s="15" t="s">
         <v>22</v>
@@ -740,7 +740,7 @@
       </c>
       <c r="K5" s="7"/>
       <c r="L5" s="12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M5" s="15" t="s">
         <v>22</v>

</xml_diff>